<commit_message>
fixed stepRemaining for Drive Mode
</commit_message>
<xml_diff>
--- a/assignment2 IR.xlsx
+++ b/assignment2 IR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring 2020\mechatronics2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E1BD6C-22A9-4E4B-91B3-2E17F6DBD53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B5DE32-7342-4039-A8A3-FFF0A189C82E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -953,50 +953,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$30:$A$42</c:f>
@@ -1052,40 +1008,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>152.53749999999999</c:v>
+                  <c:v>136.37499999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>101.82499999999999</c:v>
+                  <c:v>90.083333333333314</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.46875</c:v>
+                  <c:v>66.937499999999986</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61.254999999999995</c:v>
+                  <c:v>53.05</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.112499999999997</c:v>
+                  <c:v>43.791666666666664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.86785714285714</c:v>
+                  <c:v>37.178571428571431</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.434375000000003</c:v>
+                  <c:v>32.21875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.208333333333336</c:v>
+                  <c:v>28.361111111111114</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.827500000000001</c:v>
+                  <c:v>25.275000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.061363636363637</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.756249999999998</c:v>
+                  <c:v>20.645833333333332</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.805769230769226</c:v>
+                  <c:v>18.865384615384613</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2950,15 +2906,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>88582</xdr:rowOff>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3027,10 +2983,10 @@
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3357,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3646,8 +3602,8 @@
         <v>0.4</v>
       </c>
       <c r="B31">
-        <f>0.4+60.855/A31</f>
-        <v>152.53749999999999</v>
+        <f>55.55/A31-2.5</f>
+        <v>136.37499999999997</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -3656,8 +3612,8 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32:B42" si="2">0.4+60.855/A32</f>
-        <v>101.82499999999999</v>
+        <f t="shared" ref="B32:B42" si="2">55.55/A32-2.5</f>
+        <v>90.083333333333314</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -3667,7 +3623,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="2"/>
-        <v>76.46875</v>
+        <v>66.937499999999986</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -3677,7 +3633,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="2"/>
-        <v>61.254999999999995</v>
+        <v>53.05</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -3687,7 +3643,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="2"/>
-        <v>51.112499999999997</v>
+        <v>43.791666666666664</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -3697,7 +3653,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="2"/>
-        <v>43.86785714285714</v>
+        <v>37.178571428571431</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -3707,7 +3663,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="2"/>
-        <v>38.434375000000003</v>
+        <v>32.21875</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -3717,7 +3673,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="2"/>
-        <v>34.208333333333336</v>
+        <v>28.361111111111114</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -3727,7 +3683,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="2"/>
-        <v>30.827500000000001</v>
+        <v>25.275000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -3737,7 +3693,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="2"/>
-        <v>28.061363636363637</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -3747,7 +3703,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="2"/>
-        <v>25.756249999999998</v>
+        <v>20.645833333333332</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -3757,7 +3713,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="2"/>
-        <v>23.805769230769226</v>
+        <v>18.865384615384613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>